<commit_message>
NW Syrian sites map
</commit_message>
<xml_diff>
--- a/functions/time/Disturbances_EDTF.xlsx
+++ b/functions/time/Disturbances_EDTF.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rprojects\eamena-arches-dev\functions\time\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CEA2F6A-8509-44E4-B313-54EA1B4EC587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF803A5C-652A-4D24-AFBC-C9ACB6455F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$T$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -350,16 +353,19 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -658,16 +664,21 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B104" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M8" sqref="M8"/>
+      <selection pane="bottomRight" activeCell="H116" sqref="H116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>